<commit_message>
struggling with non-consecutive problem
</commit_message>
<xml_diff>
--- a/data/schedule.xlsx
+++ b/data/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/667b39c49d6998ed/Documents/cl_schedule/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57A5C071-0A31-45FA-9052-8EBAA64DBFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{57A5C071-0A31-45FA-9052-8EBAA64DBFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE2BB2BD-56AD-47CC-8C8F-B6C8B0954FEC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{EF90AECF-AD40-4AC8-B95F-E5CA6FF4377F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{EF90AECF-AD40-4AC8-B95F-E5CA6FF4377F}"/>
   </bookViews>
   <sheets>
     <sheet name="Days" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="34">
   <si>
     <t>Date</t>
   </si>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1A78283-7935-4C48-8F43-2124791126BD}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2178,10 +2178,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C38160A-04A3-4CDA-B574-2AE36E7D8C8E}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2282,7 +2282,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="1">
-        <v>44786</v>
+        <v>44744</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -2290,7 +2290,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="1">
-        <v>44787</v>
+        <v>44745</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -2298,7 +2298,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="1">
-        <v>44788</v>
+        <v>44786</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -2306,7 +2306,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1">
-        <v>44789</v>
+        <v>44787</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -2314,7 +2314,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="1">
-        <v>44790</v>
+        <v>44788</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -2322,7 +2322,7 @@
         <v>5</v>
       </c>
       <c r="B17" s="1">
-        <v>44791</v>
+        <v>44789</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -2330,7 +2330,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="1">
-        <v>44792</v>
+        <v>44790</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -2338,7 +2338,7 @@
         <v>5</v>
       </c>
       <c r="B19" s="1">
-        <v>44793</v>
+        <v>44791</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -2346,23 +2346,23 @@
         <v>5</v>
       </c>
       <c r="B20" s="1">
-        <v>44794</v>
+        <v>44792</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1">
-        <v>44814</v>
+        <v>44793</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B22" s="1">
-        <v>44815</v>
+        <v>44794</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -2370,7 +2370,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1">
-        <v>44816</v>
+        <v>44807</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -2378,7 +2378,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1">
-        <v>44817</v>
+        <v>44807</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -2386,7 +2386,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1">
-        <v>44818</v>
+        <v>44807</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -2394,7 +2394,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1">
-        <v>44819</v>
+        <v>44807</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -2402,7 +2402,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1">
-        <v>44820</v>
+        <v>44807</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -2410,7 +2410,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1">
-        <v>44821</v>
+        <v>44807</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -2418,12 +2418,12 @@
         <v>4</v>
       </c>
       <c r="B29" s="1">
-        <v>44822</v>
+        <v>44807</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B30" s="1">
         <v>44807</v>
@@ -2431,10 +2431,10 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B31" s="1">
-        <v>44808</v>
+        <v>44807</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -2442,7 +2442,7 @@
         <v>3</v>
       </c>
       <c r="B32" s="1">
-        <v>44809</v>
+        <v>44814</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -2450,7 +2450,7 @@
         <v>3</v>
       </c>
       <c r="B33" s="1">
-        <v>44810</v>
+        <v>44815</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -2458,7 +2458,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="1">
-        <v>44811</v>
+        <v>44816</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -2466,7 +2466,7 @@
         <v>3</v>
       </c>
       <c r="B35" s="1">
-        <v>44812</v>
+        <v>44817</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -2474,7 +2474,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="1">
-        <v>44813</v>
+        <v>44818</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -2482,7 +2482,7 @@
         <v>3</v>
       </c>
       <c r="B37" s="1">
-        <v>44814</v>
+        <v>44819</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -2490,7 +2490,23 @@
         <v>3</v>
       </c>
       <c r="B38" s="1">
-        <v>44815</v>
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="1">
+        <v>44821</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1">
+        <v>44822</v>
       </c>
     </row>
   </sheetData>

</xml_diff>